<commit_message>
Start edits of Results pages 8-10 on manuscript V1.1
</commit_message>
<xml_diff>
--- a/3-GenstatOutput/Single_vs_overlapping_QTL_enrichment.xlsx
+++ b/3-GenstatOutput/Single_vs_overlapping_QTL_enrichment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28d51258ffc36474/Juenger Projects/fourway-ionomics/3-GenstatOutput/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice\Documents\Github\fourway-ionomics\3-GenstatOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{1C4E1249-4D58-4E4E-994B-0E25F855FF03}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{22F1DD11-F0D4-4348-95CE-127DE615AFA2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6376FA-6FF6-4459-8C5D-707E2B33472F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{B2F07C1A-C0F2-4409-B87C-0BAC5E591F71}"/>
+    <workbookView xWindow="54570" yWindow="12255" windowWidth="16875" windowHeight="10530" xr2:uid="{B2F07C1A-C0F2-4409-B87C-0BAC5E591F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
-  <si>
-    <t>5 P31 single, 9 overlap</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>6 Mg26 single, 3 overlap</t>
   </si>
@@ -115,6 +115,90 @@
   </si>
   <si>
     <t>11A</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>Rb</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Mo</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>overlap</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t>macronutrient</t>
+  </si>
+  <si>
+    <t>micronutrient</t>
+  </si>
+  <si>
+    <t>non-essential analogue</t>
+  </si>
+  <si>
+    <t>harmful</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>expect 4 QTL per element, on average.</t>
+  </si>
+  <si>
+    <t>6 P31 single, 9 overlap</t>
   </si>
 </sst>
 </file>
@@ -466,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A745F7C-4E7A-4D35-9E61-069031212AE1}">
-  <dimension ref="A4:U17"/>
+  <dimension ref="A4:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -479,13 +563,13 @@
   <sheetData>
     <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -536,16 +620,16 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>9</v>
@@ -596,13 +680,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f>SUM(G4:G5)</f>
@@ -667,24 +751,24 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <f>G6*20/77</f>
@@ -745,13 +829,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <f>G6*57/77</f>
@@ -812,24 +896,24 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <f>(G4-G8)^2/G8</f>
@@ -890,13 +974,13 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <f>(G5-G9)^2/G9</f>
@@ -957,27 +1041,27 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.45">
@@ -985,38 +1069,404 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21">
+        <f>77/18</f>
+        <v>4.2777777777777777</v>
+      </c>
+      <c r="J21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23">
+        <f>SUM(C20:D23)</f>
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <f>77/(18/4)</f>
+        <v>17.111111111111111</v>
+      </c>
+      <c r="I23">
+        <f>G23/H23</f>
+        <v>0.40909090909090912</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
+      <c r="C25">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27">
+        <f>SUM(C24:D27)</f>
+        <v>36</v>
+      </c>
+      <c r="H27">
+        <f>77/(18/4)</f>
+        <v>17.111111111111111</v>
+      </c>
+      <c r="I27">
+        <f>G27/H27</f>
+        <v>2.1038961038961039</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35">
+        <f>SUM(C28:D35)</f>
+        <v>17</v>
+      </c>
+      <c r="H35">
+        <f>77/(18/8)</f>
+        <v>34.222222222222221</v>
+      </c>
+      <c r="I35">
+        <f>G35/H35</f>
+        <v>0.49675324675324678</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37">
+        <f>SUM(C36:D37)</f>
+        <v>17</v>
+      </c>
+      <c r="H37">
+        <f>77/(18/2)</f>
+        <v>8.5555555555555554</v>
+      </c>
+      <c r="I37">
+        <f>G37/H37</f>
+        <v>1.9870129870129871</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:E37">
+    <sortCondition ref="E20:E37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish edits of Results section and add Discussion point ideas
</commit_message>
<xml_diff>
--- a/3-GenstatOutput/Single_vs_overlapping_QTL_enrichment.xlsx
+++ b/3-GenstatOutput/Single_vs_overlapping_QTL_enrichment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice\Documents\Github\fourway-ionomics\3-GenstatOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6376FA-6FF6-4459-8C5D-707E2B33472F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B8F023-8F64-4A9E-B052-0C1F56F9DED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54570" yWindow="12255" windowWidth="16875" windowHeight="10530" xr2:uid="{B2F07C1A-C0F2-4409-B87C-0BAC5E591F71}"/>
+    <workbookView xWindow="44880" yWindow="7755" windowWidth="29040" windowHeight="15840" xr2:uid="{B2F07C1A-C0F2-4409-B87C-0BAC5E591F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="72">
   <si>
     <t>6 Mg26 single, 3 overlap</t>
   </si>
@@ -78,9 +78,6 @@
     <t>More Mg26 singletons than expected</t>
   </si>
   <si>
-    <t>Fewer Ca44 singletons than expected, and fewer Al27 singletons than expected</t>
-  </si>
-  <si>
     <t>need</t>
   </si>
   <si>
@@ -199,6 +196,60 @@
   </si>
   <si>
     <t>6 P31 single, 9 overlap</t>
+  </si>
+  <si>
+    <t>Fewer Ca, Mn, and Al singletons than expected</t>
+  </si>
+  <si>
+    <t>bioavailable</t>
+  </si>
+  <si>
+    <t>zero to VI, VI most common</t>
+  </si>
+  <si>
+    <t>ince then, iron in biological molecules has been progressively substituted by Cu which is able to perform similar functions. T</t>
+  </si>
+  <si>
+    <t>2+</t>
+  </si>
+  <si>
+    <t>2+ or 3+</t>
+  </si>
+  <si>
+    <t>3- phosphate</t>
+  </si>
+  <si>
+    <t>3+</t>
+  </si>
+  <si>
+    <t>1+</t>
+  </si>
+  <si>
+    <t>1+ or 2+</t>
+  </si>
+  <si>
+    <t>zero to VI</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>analogue</t>
+  </si>
+  <si>
+    <t>most common: 1+</t>
+  </si>
+  <si>
+    <t>15 total</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>exp</t>
   </si>
 </sst>
 </file>
@@ -234,8 +285,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A745F7C-4E7A-4D35-9E61-069031212AE1}">
-  <dimension ref="A4:U37"/>
+  <dimension ref="A3:V55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -561,15 +613,59 @@
     <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -593,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -615,21 +711,21 @@
       </c>
       <c r="U4">
         <f>SUM(G4:T4)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>9</v>
@@ -653,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="N5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O5">
         <v>4</v>
@@ -675,15 +771,15 @@
       </c>
       <c r="U5">
         <f>SUM(G5:T5)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -751,10 +847,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -762,10 +858,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -829,10 +925,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -896,10 +992,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -907,10 +1003,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -920,11 +1016,11 @@
         <v>0.51136363636363646</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:T11" si="3">(H4-H8)^2/H8</f>
+        <f>(H4-H8)^2/H8</f>
         <v>5.7376623376623384</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I11:T11" si="3">(I4-I8)^2/I8</f>
         <v>4.8773448773448747E-2</v>
       </c>
       <c r="J11">
@@ -945,7 +1041,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>1.2987012987012987</v>
+        <v>6.8701298701298694E-2</v>
       </c>
       <c r="O11">
         <f t="shared" si="3"/>
@@ -974,10 +1070,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1012,7 +1108,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>0.45568466621098197</v>
+        <v>2.4105718842560946E-2</v>
       </c>
       <c r="O12">
         <f t="shared" si="4"/>
@@ -1041,10 +1137,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1052,10 +1148,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -1069,403 +1165,1023 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="O16" t="s">
+        <v>66</v>
+      </c>
+      <c r="P16" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>26</v>
+      </c>
+      <c r="R16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" t="s">
+        <v>30</v>
+      </c>
+      <c r="T16" t="s">
+        <v>63</v>
+      </c>
+      <c r="U16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C19" t="s">
+      <c r="P17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" t="s">
+        <v>62</v>
+      </c>
+      <c r="U18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="P19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>26</v>
+      </c>
+      <c r="R19" t="s">
+        <v>33</v>
+      </c>
+      <c r="T19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" t="s">
+        <v>47</v>
+      </c>
+      <c r="P20" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q20" t="s">
         <v>26</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="R20" t="s">
+        <v>38</v>
+      </c>
+      <c r="S20" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" t="s">
+        <v>64</v>
+      </c>
+      <c r="U20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>4</v>
       </c>
-      <c r="E21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21">
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21">
         <f>77/18</f>
         <v>4.2777777777777777</v>
       </c>
-      <c r="J21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K21" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" t="s">
+        <v>66</v>
+      </c>
+      <c r="P21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>26</v>
+      </c>
+      <c r="R21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
       </c>
       <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" t="s">
         <v>51</v>
       </c>
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="O22" t="s">
+        <v>66</v>
+      </c>
+      <c r="P22" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>31</v>
+      </c>
+      <c r="R22" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>43</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23">
-        <f>SUM(C20:D23)</f>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23">
+        <f>SUM(D20:E23)</f>
         <v>7</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f>77/(18/4)</f>
         <v>17.111111111111111</v>
       </c>
-      <c r="I23">
-        <f>G23/H23</f>
+      <c r="J23">
+        <f>H23/I23</f>
         <v>0.40909090909090912</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="O23" t="s">
+        <v>66</v>
+      </c>
+      <c r="P23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>26</v>
+      </c>
+      <c r="R23" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" t="s">
+        <v>30</v>
+      </c>
+      <c r="T23" t="s">
+        <v>62</v>
+      </c>
+      <c r="U23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" t="s">
+        <v>31</v>
+      </c>
+      <c r="T24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24">
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25">
         <v>6</v>
       </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="P26" t="s">
         <v>31</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
+      <c r="Q26" t="s">
+        <v>33</v>
+      </c>
+      <c r="T26" t="s">
+        <v>62</v>
+      </c>
+      <c r="U26" t="s">
+        <v>58</v>
+      </c>
+      <c r="V26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27">
-        <f>SUM(C24:D27)</f>
+      <c r="F27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27">
+        <f>SUM(D24:E27)</f>
         <v>36</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f>77/(18/4)</f>
         <v>17.111111111111111</v>
       </c>
-      <c r="I27">
-        <f>G27/H27</f>
+      <c r="J27">
+        <f>H27/I27</f>
         <v>2.1038961038961039</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>59</v>
+      </c>
+      <c r="O27" t="s">
+        <v>58</v>
+      </c>
+      <c r="P27" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>58</v>
+      </c>
+      <c r="T27">
+        <v>1.5</v>
+      </c>
+      <c r="U27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>45</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
         <v>20</v>
       </c>
-      <c r="C28">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="U30">
         <v>1</v>
       </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" t="s">
+        <v>68</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31">
-        <v>8</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>42</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="E33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N33" t="s">
+        <v>62</v>
+      </c>
+      <c r="O33" t="s">
+        <v>59</v>
+      </c>
+      <c r="P33" t="s">
+        <v>61</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>45</v>
+      </c>
+      <c r="T34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
         <v>49</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35">
-        <f>SUM(C28:D35)</f>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35">
+        <f>SUM(D28:E35)</f>
         <v>17</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <f>77/(18/8)</f>
         <v>34.222222222222221</v>
       </c>
-      <c r="I35">
-        <f>G35/H35</f>
+      <c r="J35">
+        <f>H35/I35</f>
         <v>0.49675324675324678</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="M35" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35" t="s">
+        <v>31</v>
+      </c>
+      <c r="O35" t="s">
+        <v>28</v>
+      </c>
+      <c r="P35" t="s">
+        <v>29</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+      <c r="M36" t="s">
+        <v>58</v>
+      </c>
+      <c r="N36" t="s">
+        <v>58</v>
+      </c>
+      <c r="O36" t="s">
+        <v>58</v>
+      </c>
+      <c r="P36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>7</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37">
         <v>3</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>5</v>
       </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
-      <c r="G37">
-        <f>SUM(C36:D37)</f>
+      <c r="F37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37">
+        <f>SUM(D36:E37)</f>
         <v>17</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <f>77/(18/2)</f>
         <v>8.5555555555555554</v>
       </c>
-      <c r="I37">
-        <f>G37/H37</f>
+      <c r="J37">
+        <f>H37/I37</f>
         <v>1.9870129870129871</v>
       </c>
+      <c r="S37" t="s">
+        <v>70</v>
+      </c>
+      <c r="T37">
+        <v>8.5</v>
+      </c>
+      <c r="U37">
+        <v>6.5</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="V38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="S39" t="s">
+        <v>71</v>
+      </c>
+      <c r="T39">
+        <f>O55*15</f>
+        <v>5.2325581395348841</v>
+      </c>
+      <c r="U39">
+        <f>P55*15</f>
+        <v>8.0232558139534884</v>
+      </c>
+      <c r="V39">
+        <f>Q55*15</f>
+        <v>1.7441860465116279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="O40" t="s">
+        <v>62</v>
+      </c>
+      <c r="P40" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <f>(T37-T39)^2/T39</f>
+        <v>2.0403359173126607</v>
+      </c>
+      <c r="U41">
+        <f>(U37-U39)^2/U39</f>
+        <v>0.28919784293899564</v>
+      </c>
+      <c r="V41">
+        <f>(V37-V39)^2/V39</f>
+        <v>1.7441860465116279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="P43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="E44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" t="s">
+        <v>33</v>
+      </c>
+      <c r="I44" t="s">
+        <v>27</v>
+      </c>
+      <c r="P44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H46" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" t="s">
+        <v>34</v>
+      </c>
+      <c r="K46" t="s">
+        <v>33</v>
+      </c>
+      <c r="O46">
+        <v>2</v>
+      </c>
+      <c r="P46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="P47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
+      </c>
+      <c r="F48" t="s">
+        <v>61</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" t="s">
+        <v>30</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="O50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51">
+        <v>3.5</v>
+      </c>
+      <c r="F51">
+        <v>1.5</v>
+      </c>
+      <c r="P51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="O52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53">
+        <f>O55*9</f>
+        <v>3.1395348837209305</v>
+      </c>
+      <c r="E53">
+        <f>P55*9</f>
+        <v>4.8139534883720927</v>
+      </c>
+      <c r="F53">
+        <f>Q55*9</f>
+        <v>1.0465116279069768</v>
+      </c>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="O54">
+        <v>15</v>
+      </c>
+      <c r="P54">
+        <v>23</v>
+      </c>
+      <c r="Q54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="D55">
+        <f>(D51-D53)^2/D53</f>
+        <v>3.1395348837209309</v>
+      </c>
+      <c r="E55">
+        <f>(E51-E53)^2/E53</f>
+        <v>0.35863947871025709</v>
+      </c>
+      <c r="F55">
+        <f>(F51-F53)^2/F53</f>
+        <v>0.19651162790697665</v>
+      </c>
+      <c r="O55">
+        <f>15/(15+23+5)</f>
+        <v>0.34883720930232559</v>
+      </c>
+      <c r="P55">
+        <f>23/(15+23+5)</f>
+        <v>0.53488372093023251</v>
+      </c>
+      <c r="Q55">
+        <f>5/(15+23+5)</f>
+        <v>0.11627906976744186</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:E37">
-    <sortCondition ref="E20:E37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B20:F37">
+    <sortCondition ref="F20:F37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>